<commit_message>
Update Mind maps and Table Mockups - model3 without NLP features actually has the best performance by almost 20%?
</commit_message>
<xml_diff>
--- a/Code/Modelling/Logistic Regression/Table Mockups.xlsx
+++ b/Code/Modelling/Logistic Regression/Table Mockups.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ijyli\repo\Stat-222-Project\Code\Modelling\Logistic Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Stat-222-Project\Code\Modelling\Logistic Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178DB971-4A1D-4717-86F8-D89A38CAC584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32643427-2820-4F77-A0FE-1A957BA3792A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{3D2C448C-6442-4295-93EC-799C28269F03}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{3D2C448C-6442-4295-93EC-799C28269F03}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Comparison Table" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="39">
   <si>
     <t>Change in Rating Model</t>
   </si>
@@ -132,15 +132,54 @@
   </si>
   <si>
     <t>Solver</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>F1-Score</t>
+  </si>
+  <si>
+    <t>1. AltmanZ as the Only Covariate</t>
+  </si>
+  <si>
+    <t>0. Majority Baseline</t>
+  </si>
+  <si>
+    <t>2. All Numerical Financial Features</t>
+  </si>
+  <si>
+    <t>5. Categorical + Numerical + NLP Features</t>
+  </si>
+  <si>
+    <t>4. Categorical and Numerical Features</t>
+  </si>
+  <si>
+    <t>3. NLP and Numerical Financial Features</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -155,7 +194,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -163,20 +202,332 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -187,6 +538,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A12507FE-3B56-49DE-BEFC-0D73B35FC20A}" name="Table3" displayName="Table3" ref="A3:E9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
+  <autoFilter ref="A3:E9" xr:uid="{A12507FE-3B56-49DE-BEFC-0D73B35FC20A}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2E6DF127-8867-4AEE-B8F0-EF92156A6803}" name="Models" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{187D12AE-9765-4129-91D8-61A2DC0AEC21}" name="Precision" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{DEC3CA8A-57B9-48C4-A610-459CC16159A3}" name="Recall" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{176C630D-EBC7-4547-BE5D-B789261E5428}" name="F1-Score" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{B5ADF4C5-8230-4D6D-A2BC-AA290C672DC4}" name="Accuracy" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -985,43 +1356,152 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52E18D-FE45-4C7C-927C-059F651F77F3}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="12">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.43</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0.49</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0.51</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.45</v>
+      </c>
+      <c r="E6" s="15">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0.59</v>
+      </c>
+      <c r="C7" s="15">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E7" s="15">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0.95</v>
+      </c>
+      <c r="C8" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="E8" s="15">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0.77</v>
+      </c>
+      <c r="C9" s="15">
+        <v>0.78</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.77</v>
+      </c>
+      <c r="E9" s="15">
+        <v>0.78</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rearranged some cells (lasso path was actually computed on a model with nlp + numerical financial)
</commit_message>
<xml_diff>
--- a/Code/Modelling/Logistic Regression/Table Mockups.xlsx
+++ b/Code/Modelling/Logistic Regression/Table Mockups.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Stat-222-Project\Code\Modelling\Logistic Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32643427-2820-4F77-A0FE-1A957BA3792A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C1E4D4-9255-4375-90DC-D9B1AEA774A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{3D2C448C-6442-4295-93EC-799C28269F03}"/>
   </bookViews>
@@ -322,15 +322,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -349,7 +340,7 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -358,7 +349,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -366,45 +366,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -506,13 +467,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -525,6 +479,52 @@
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -541,7 +541,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A12507FE-3B56-49DE-BEFC-0D73B35FC20A}" name="Table3" displayName="Table3" ref="A3:E9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A12507FE-3B56-49DE-BEFC-0D73B35FC20A}" name="Table3" displayName="Table3" ref="A3:E9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
   <autoFilter ref="A3:E9" xr:uid="{A12507FE-3B56-49DE-BEFC-0D73B35FC20A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -550,11 +550,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2E6DF127-8867-4AEE-B8F0-EF92156A6803}" name="Models" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{187D12AE-9765-4129-91D8-61A2DC0AEC21}" name="Precision" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{DEC3CA8A-57B9-48C4-A610-459CC16159A3}" name="Recall" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{176C630D-EBC7-4547-BE5D-B789261E5428}" name="F1-Score" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{B5ADF4C5-8230-4D6D-A2BC-AA290C672DC4}" name="Accuracy" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{2E6DF127-8867-4AEE-B8F0-EF92156A6803}" name="Models" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{187D12AE-9765-4129-91D8-61A2DC0AEC21}" name="Precision" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DEC3CA8A-57B9-48C4-A610-459CC16159A3}" name="Recall" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{176C630D-EBC7-4547-BE5D-B789261E5428}" name="F1-Score" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{B5ADF4C5-8230-4D6D-A2BC-AA290C672DC4}" name="Accuracy" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1375,124 +1375,124 @@
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="12">
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9">
         <v>0.32</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="8">
         <v>0.4</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>0.43</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <v>0.4</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>0.43</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="11">
         <v>0.49</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>0.51</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>0.45</v>
       </c>
-      <c r="E6" s="15">
-        <v>0.51</v>
+      <c r="E6" s="12">
+        <v>0.50900000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="11">
         <v>0.59</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="7">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E7" s="15">
-        <v>0.56999999999999995</v>
+      <c r="E7" s="12">
+        <v>0.57499999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="11">
         <v>0.95</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>0.95</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <v>0.95</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="12">
+        <v>0.95199999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="11">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="14">
-        <v>0.77</v>
-      </c>
-      <c r="C9" s="15">
-        <v>0.78</v>
-      </c>
-      <c r="D9" s="10">
-        <v>0.77</v>
-      </c>
-      <c r="E9" s="15">
-        <v>0.78</v>
+      <c r="C9" s="12">
+        <v>0.95</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.95399999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>